<commit_message>
agregado paneles ica-sfe, globales mensuales y globales trimestrales terminados previsionalmente
</commit_message>
<xml_diff>
--- a/web_ces/Paneles/global_trimestral/input/Clasificador.xlsx
+++ b/web_ces/Paneles/global_trimestral/input/Clasificador.xlsx
@@ -512,8 +512,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5178340cf401e55f52edc65754db13eb">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f34c51a0a6f5e7009dcf60732b5bba38" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="126bfeb7ae601119bfc9c37fe78f3e1b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2137ec74e9b380cd6ab08453deebfc43" ns2:_="" ns3:_="">
     <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
     <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
     <xsd:element name="properties">
@@ -732,7 +732,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC086DC-C13B-4AB5-8D03-1EED5AA52344}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{870E25B7-AE41-4B13-8A66-4CA6FFDDD01E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
agregado calendario V2 provisorio
</commit_message>
<xml_diff>
--- a/web_ces/Paneles/global_trimestral/input/Clasificador.xlsx
+++ b/web_ces/Paneles/global_trimestral/input/Clasificador.xlsx
@@ -512,8 +512,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5178340cf401e55f52edc65754db13eb">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f34c51a0a6f5e7009dcf60732b5bba38" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C5B9F2161CEE1040BBC03CB11300495F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="126bfeb7ae601119bfc9c37fe78f3e1b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5dd4176-d247-4204-85b8-921214f3ccea" xmlns:ns3="359b39ce-e1f9-4933-8424-33b611e6fdcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2137ec74e9b380cd6ab08453deebfc43" ns2:_="" ns3:_="">
     <xsd:import namespace="b5dd4176-d247-4204-85b8-921214f3ccea"/>
     <xsd:import namespace="359b39ce-e1f9-4933-8424-33b611e6fdcd"/>
     <xsd:element name="properties">
@@ -732,7 +732,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC086DC-C13B-4AB5-8D03-1EED5AA52344}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09DDB38D-3128-4461-81B1-1CEB10BE6D2D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>